<commit_message>
json és emailes gombok működnek, json beégetve emailbe
</commit_message>
<xml_diff>
--- a/public/mailDatas.xlsx
+++ b/public/mailDatas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MUNKA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MUNKA\email_AKK\web\html\emailKuldoProg\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DA02207A-0660-4D94-883A-252D1C601DA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16DBC608-E08C-47B8-A4D1-A5941FBD8F60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3540" yWindow="2295" windowWidth="21600" windowHeight="11325"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="mailDatas" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>Név</t>
   </si>
@@ -56,12 +56,30 @@
   </si>
   <si>
     <t>Hatodik Helén</t>
+  </si>
+  <si>
+    <t>00524</t>
+  </si>
+  <si>
+    <t>00525</t>
+  </si>
+  <si>
+    <t>00526</t>
+  </si>
+  <si>
+    <t>00527</t>
+  </si>
+  <si>
+    <t>00528</t>
+  </si>
+  <si>
+    <t>00529</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -557,8 +575,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - 1. jelölőszín" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -933,12 +952,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -955,8 +979,8 @@
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2">
-        <v>524</v>
+      <c r="B2" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -966,8 +990,8 @@
       <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3">
-        <v>525</v>
+      <c r="B3" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
@@ -977,8 +1001,8 @@
       <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B4">
-        <v>526</v>
+      <c r="B4" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
@@ -988,8 +1012,8 @@
       <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="B5">
-        <v>527</v>
+      <c r="B5" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
@@ -999,8 +1023,8 @@
       <c r="A6" t="s">
         <v>10</v>
       </c>
-      <c r="B6">
-        <v>528</v>
+      <c r="B6" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="C6" t="s">
         <v>7</v>
@@ -1010,8 +1034,8 @@
       <c r="A7" t="s">
         <v>11</v>
       </c>
-      <c r="B7">
-        <v>529</v>
+      <c r="B7" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>

</xml_diff>